<commit_message>
releasing version 1 of the APIs
</commit_message>
<xml_diff>
--- a/db/data_model.xlsx
+++ b/db/data_model.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\Bootcamp\surveySquid\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\Bootcamp\surveySquid\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="19560" windowHeight="8205"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="19560" windowHeight="8205"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,9 +65,6 @@
     <t>survey_end_date</t>
   </si>
   <si>
-    <t>public, group</t>
-  </si>
-  <si>
     <t>SURVEY_QUESTION</t>
   </si>
   <si>
@@ -138,6 +135,9 @@
   </si>
   <si>
     <t>INT(5)</t>
+  </si>
+  <si>
+    <t>public, private</t>
   </si>
 </sst>
 </file>
@@ -246,13 +246,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -548,7 +548,7 @@
   <dimension ref="A2:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -572,49 +572,49 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
       <c r="E2" s="7" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
       <c r="I2" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J2" s="9"/>
       <c r="K2" s="10"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="C3" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="G3" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="G3" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="K3" s="5" t="s">
         <v>27</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -622,21 +622,21 @@
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C4" s="1"/>
       <c r="E4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G4" s="1"/>
       <c r="I4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K4" s="1"/>
     </row>
@@ -645,21 +645,21 @@
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" s="1"/>
       <c r="E5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G5" s="1"/>
       <c r="I5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K5" s="1"/>
     </row>
@@ -668,21 +668,21 @@
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C6" s="1"/>
       <c r="E6" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G6" s="1"/>
       <c r="I6" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>10</v>
@@ -693,23 +693,23 @@
         <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7" s="1"/>
       <c r="E7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K7" s="1"/>
     </row>
@@ -718,14 +718,14 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C8" s="1"/>
       <c r="E8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G8" s="1"/>
     </row>
@@ -734,101 +734,101 @@
         <v>12</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G9" s="1"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
       <c r="D12" s="2"/>
       <c r="E12" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="C13" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>28</v>
-      </c>
       <c r="D13" s="3"/>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="G13" s="5" t="s">
         <v>27</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="3"/>
       <c r="E14" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="3"/>
       <c r="E15" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G15" s="1"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="3"/>
       <c r="E16" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G16" s="1"/>
     </row>
     <row r="17" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E17" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G17" s="1"/>
     </row>

</xml_diff>